<commit_message>
fix two missing CDS/exon index in CBS432
</commit_message>
<xml_diff>
--- a/data_20170128/Supplementary_Data_Sets/PRJEB7245_strain_read_mapping.xlsx
+++ b/data_20170128/Supplementary_Data_Sets/PRJEB7245_strain_read_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="1900" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="277">
   <si>
     <t>DBVPG6044</t>
   </si>
@@ -370,6 +370,489 @@
   </si>
   <si>
     <t>Strain-sample mapping for PacBio reads generated in the study PRJEB7245 (URL: http://www.ebi.ac.uk/ena/data/view/PRJEB7245)</t>
+  </si>
+  <si>
+    <t>ENA secondary sample accession</t>
+  </si>
+  <si>
+    <t>Experimental accession</t>
+  </si>
+  <si>
+    <t>Run accession</t>
+  </si>
+  <si>
+    <t>ERX1095601</t>
+  </si>
+  <si>
+    <t>ERR1016541</t>
+  </si>
+  <si>
+    <t>ERS542092</t>
+  </si>
+  <si>
+    <t>ERX1095602</t>
+  </si>
+  <si>
+    <t>ERR1016542</t>
+  </si>
+  <si>
+    <t>ERX1104159</t>
+  </si>
+  <si>
+    <t>ERR1025287</t>
+  </si>
+  <si>
+    <t>ERX1104160</t>
+  </si>
+  <si>
+    <t>ERR1025288</t>
+  </si>
+  <si>
+    <t>ERS542096</t>
+  </si>
+  <si>
+    <t>ERX1160112</t>
+  </si>
+  <si>
+    <t>ERR1080522</t>
+  </si>
+  <si>
+    <t>ERS542097</t>
+  </si>
+  <si>
+    <t>ERX1160113</t>
+  </si>
+  <si>
+    <t>ERR1080523</t>
+  </si>
+  <si>
+    <t>ERS542098</t>
+  </si>
+  <si>
+    <t>ERX1160114</t>
+  </si>
+  <si>
+    <t>ERR1080524</t>
+  </si>
+  <si>
+    <t>ERS542093</t>
+  </si>
+  <si>
+    <t>ERX1160115</t>
+  </si>
+  <si>
+    <t>ERR1080525</t>
+  </si>
+  <si>
+    <t>ERS542094</t>
+  </si>
+  <si>
+    <t>ERX1160116</t>
+  </si>
+  <si>
+    <t>ERR1080526</t>
+  </si>
+  <si>
+    <t>ERS542100</t>
+  </si>
+  <si>
+    <t>ERX1160117</t>
+  </si>
+  <si>
+    <t>ERR1080527</t>
+  </si>
+  <si>
+    <t>ERS542101</t>
+  </si>
+  <si>
+    <t>ERX1160118</t>
+  </si>
+  <si>
+    <t>ERR1080528</t>
+  </si>
+  <si>
+    <t>ERX1160119</t>
+  </si>
+  <si>
+    <t>ERR1080529</t>
+  </si>
+  <si>
+    <t>ERX1160120</t>
+  </si>
+  <si>
+    <t>ERR1080530</t>
+  </si>
+  <si>
+    <t>ERX1160121</t>
+  </si>
+  <si>
+    <t>ERR1080531</t>
+  </si>
+  <si>
+    <t>ERX1160122</t>
+  </si>
+  <si>
+    <t>ERR1080532</t>
+  </si>
+  <si>
+    <t>ERX1160123</t>
+  </si>
+  <si>
+    <t>ERR1080533</t>
+  </si>
+  <si>
+    <t>ERX1160124</t>
+  </si>
+  <si>
+    <t>ERR1080534</t>
+  </si>
+  <si>
+    <t>ERX1160125</t>
+  </si>
+  <si>
+    <t>ERR1080535</t>
+  </si>
+  <si>
+    <t>ERX1160126</t>
+  </si>
+  <si>
+    <t>ERR1080536</t>
+  </si>
+  <si>
+    <t>ERX1160127</t>
+  </si>
+  <si>
+    <t>ERR1080537</t>
+  </si>
+  <si>
+    <t>ERX1160128</t>
+  </si>
+  <si>
+    <t>ERR1080538</t>
+  </si>
+  <si>
+    <t>ERX1160129</t>
+  </si>
+  <si>
+    <t>ERR1080539</t>
+  </si>
+  <si>
+    <t>ERX1160130</t>
+  </si>
+  <si>
+    <t>ERR1080540</t>
+  </si>
+  <si>
+    <t>ERX1160131</t>
+  </si>
+  <si>
+    <t>ERR1080541</t>
+  </si>
+  <si>
+    <t>ERX1160132</t>
+  </si>
+  <si>
+    <t>ERR1080542</t>
+  </si>
+  <si>
+    <t>ERX1160133</t>
+  </si>
+  <si>
+    <t>ERR1080543</t>
+  </si>
+  <si>
+    <t>ERX1180331</t>
+  </si>
+  <si>
+    <t>ERR1100797</t>
+  </si>
+  <si>
+    <t>ERX1188862</t>
+  </si>
+  <si>
+    <t>ERR1109331</t>
+  </si>
+  <si>
+    <t>ERX1203441</t>
+  </si>
+  <si>
+    <t>ERS542095</t>
+  </si>
+  <si>
+    <t>ERR1124242</t>
+  </si>
+  <si>
+    <t>ERX1203442</t>
+  </si>
+  <si>
+    <t>ERR1124243</t>
+  </si>
+  <si>
+    <t>ERX1203443</t>
+  </si>
+  <si>
+    <t>ERR1124244</t>
+  </si>
+  <si>
+    <t>ERX1203444</t>
+  </si>
+  <si>
+    <t>ERR1124245</t>
+  </si>
+  <si>
+    <t>ERX1219824</t>
+  </si>
+  <si>
+    <t>ERR1140975</t>
+  </si>
+  <si>
+    <t>ERX1219825</t>
+  </si>
+  <si>
+    <t>ERR1140976</t>
+  </si>
+  <si>
+    <t>ERX1219826</t>
+  </si>
+  <si>
+    <t>ERR1140977</t>
+  </si>
+  <si>
+    <t>ERX1219827</t>
+  </si>
+  <si>
+    <t>ERR1140978</t>
+  </si>
+  <si>
+    <t>ERX1219828</t>
+  </si>
+  <si>
+    <t>ERR1140979</t>
+  </si>
+  <si>
+    <t>ERX1219829</t>
+  </si>
+  <si>
+    <t>ERR1140980</t>
+  </si>
+  <si>
+    <t>ERX1219830</t>
+  </si>
+  <si>
+    <t>ERR1140981</t>
+  </si>
+  <si>
+    <t>ERX1266672</t>
+  </si>
+  <si>
+    <t>ERR1193288</t>
+  </si>
+  <si>
+    <t>ERX1283068</t>
+  </si>
+  <si>
+    <t>ERR1210826</t>
+  </si>
+  <si>
+    <t>ERX1725434</t>
+  </si>
+  <si>
+    <t>ERR1655118</t>
+  </si>
+  <si>
+    <t>ERS1360911</t>
+  </si>
+  <si>
+    <t>ERX1725435</t>
+  </si>
+  <si>
+    <t>ERR1655119</t>
+  </si>
+  <si>
+    <t>ERX1725436</t>
+  </si>
+  <si>
+    <t>ERS1360912</t>
+  </si>
+  <si>
+    <t>ERR1655120</t>
+  </si>
+  <si>
+    <t>ERX1725437</t>
+  </si>
+  <si>
+    <t>ERR1655121</t>
+  </si>
+  <si>
+    <t>ERS1360910</t>
+  </si>
+  <si>
+    <t>ERX1725438</t>
+  </si>
+  <si>
+    <t>ERR1655122</t>
+  </si>
+  <si>
+    <t>ERX558414</t>
+  </si>
+  <si>
+    <t>ERR601585</t>
+  </si>
+  <si>
+    <t>ERX558415</t>
+  </si>
+  <si>
+    <t>ERR601586</t>
+  </si>
+  <si>
+    <t>ERX558416</t>
+  </si>
+  <si>
+    <t>ERR601587</t>
+  </si>
+  <si>
+    <t>ERX558417</t>
+  </si>
+  <si>
+    <t>ERR601588</t>
+  </si>
+  <si>
+    <t>ERX558418</t>
+  </si>
+  <si>
+    <t>ERR601589</t>
+  </si>
+  <si>
+    <t>ERX558419</t>
+  </si>
+  <si>
+    <t>ERR601590</t>
+  </si>
+  <si>
+    <t>ERX558420</t>
+  </si>
+  <si>
+    <t>ERR601591</t>
+  </si>
+  <si>
+    <t>ERX558421</t>
+  </si>
+  <si>
+    <t>ERR601592</t>
+  </si>
+  <si>
+    <t>ERX558422</t>
+  </si>
+  <si>
+    <t>ERR601593</t>
+  </si>
+  <si>
+    <t>ERX558425</t>
+  </si>
+  <si>
+    <t>ERR601596</t>
+  </si>
+  <si>
+    <t>ERX558426</t>
+  </si>
+  <si>
+    <t>ERR601597</t>
+  </si>
+  <si>
+    <t>ERX558427</t>
+  </si>
+  <si>
+    <t>ERR601598</t>
+  </si>
+  <si>
+    <t>ERX558428</t>
+  </si>
+  <si>
+    <t>ERR601599</t>
+  </si>
+  <si>
+    <t>ERX558429</t>
+  </si>
+  <si>
+    <t>ERR601600</t>
+  </si>
+  <si>
+    <t>ERX558430</t>
+  </si>
+  <si>
+    <t>ERR601601</t>
+  </si>
+  <si>
+    <t>ERX558431</t>
+  </si>
+  <si>
+    <t>ERR601602</t>
+  </si>
+  <si>
+    <t>ERX558432</t>
+  </si>
+  <si>
+    <t>ERR601603</t>
+  </si>
+  <si>
+    <t>ERX558433</t>
+  </si>
+  <si>
+    <t>ERR601604</t>
+  </si>
+  <si>
+    <t>ERX558434</t>
+  </si>
+  <si>
+    <t>ERR601605</t>
+  </si>
+  <si>
+    <t>ERX558435</t>
+  </si>
+  <si>
+    <t>ERR601606</t>
+  </si>
+  <si>
+    <t>ERX1066581</t>
+  </si>
+  <si>
+    <t>ERR985360</t>
+  </si>
+  <si>
+    <t>ERX1066582</t>
+  </si>
+  <si>
+    <t>ERR985361</t>
+  </si>
+  <si>
+    <t>ERX558406</t>
+  </si>
+  <si>
+    <t>ERR601577</t>
+  </si>
+  <si>
+    <t>ERX558407</t>
+  </si>
+  <si>
+    <t>ERR601578</t>
+  </si>
+  <si>
+    <t>ERX558408</t>
+  </si>
+  <si>
+    <t>ERR601579</t>
+  </si>
+  <si>
+    <t>ERX558409</t>
+  </si>
+  <si>
+    <t>ERR601580</t>
+  </si>
+  <si>
+    <t>ERX558410</t>
+  </si>
+  <si>
+    <t>ERR601581</t>
   </si>
 </sst>
 </file>
@@ -460,7 +943,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -660,8 +1143,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -672,8 +1157,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -773,6 +1259,8 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1206,26 +1694,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="65.83203125" customWidth="1"/>
+    <col min="3" max="6" width="19.83203125" customWidth="1"/>
+    <col min="7" max="7" width="65.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -1236,13 +1724,22 @@
         <v>107</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>111</v>
       </c>
@@ -1253,24 +1750,39 @@
         <v>46</v>
       </c>
       <c r="D4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="D5" t="s">
+    <row r="5" spans="1:11">
+      <c r="G5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="D6" t="s">
+    <row r="6" spans="1:11">
+      <c r="E6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
         <v>0</v>
@@ -1278,58 +1790,116 @@
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="D8" s="4" t="s">
+    <row r="8" spans="1:11">
+      <c r="E8" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="D9" s="1" t="s">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="D10" s="1" t="s">
+    <row r="10" spans="1:11">
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:11">
+      <c r="E11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="D12" s="1" t="s">
+    <row r="12" spans="1:11">
+      <c r="E12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="D13" s="1" t="s">
+    <row r="13" spans="1:11">
+      <c r="E13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="D14" s="1" t="s">
+    <row r="14" spans="1:11">
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="D15" s="1" t="s">
+    <row r="15" spans="1:11">
+      <c r="E15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:11">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="s">
         <v>1</v>
@@ -1337,56 +1907,103 @@
       <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="H16" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="D17" s="4" t="s">
+    <row r="17" spans="1:8">
+      <c r="E17" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="D18" s="4" t="s">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="E18" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="D19" s="4" t="s">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="E19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="D20" s="4" t="s">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="E20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="D21" s="1" t="s">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="D22" s="1" t="s">
+    <row r="22" spans="1:8">
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="D23" s="1" t="s">
+    <row r="23" spans="1:8">
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:8">
       <c r="A24" s="3"/>
       <c r="B24" s="7" t="s">
         <v>2</v>
@@ -1394,239 +2011,455 @@
       <c r="C24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="H24" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="D25" s="4" t="s">
+    <row r="25" spans="1:8">
+      <c r="G25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="D26" s="4" t="s">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="G26" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="D27" s="1" t="s">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="D28" s="1" t="s">
+    <row r="28" spans="1:8">
+      <c r="E28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="D29" s="1" t="s">
+    <row r="29" spans="1:8">
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="D30" s="1" t="s">
+    <row r="30" spans="1:8">
+      <c r="E30" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="D31" s="1" t="s">
+    <row r="31" spans="1:8">
+      <c r="E31" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="D32" s="1" t="s">
+    <row r="32" spans="1:8">
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" t="s">
+        <v>199</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:8">
       <c r="B33" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="H33" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
-      <c r="D34" s="4" t="s">
+    <row r="34" spans="2:8">
+      <c r="E34" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="D35" s="4" t="s">
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="E35" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="D36" t="s">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" t="s">
         <v>82</v>
       </c>
-      <c r="E36" t="s">
+      <c r="H36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="D37" t="s">
+    <row r="37" spans="2:8">
+      <c r="E37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
-      <c r="D38" t="s">
+    <row r="38" spans="2:8">
+      <c r="E38" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" t="s">
+        <v>170</v>
+      </c>
+      <c r="G38" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="D39" t="s">
+    <row r="39" spans="2:8">
+      <c r="E39" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
-      <c r="D40" t="s">
+    <row r="40" spans="2:8">
+      <c r="E40" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" t="s">
+        <v>201</v>
+      </c>
+      <c r="G40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:8">
       <c r="B41" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="H41" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
-      <c r="D42" s="4" t="s">
+    <row r="42" spans="2:8">
+      <c r="E42" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="D43" s="4" t="s">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="E43" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="D44" s="4" t="s">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="E44" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="D45" s="4" t="s">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="E45" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="G45" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="D46" s="4" t="s">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="E46" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="D47" s="4" t="s">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="E47" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="D48" t="s">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="E48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F48" t="s">
+        <v>148</v>
+      </c>
+      <c r="G48" t="s">
         <v>95</v>
       </c>
-      <c r="E48" t="s">
+      <c r="H48" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="D49" t="s">
+    <row r="49" spans="1:8">
+      <c r="E49" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" t="s">
+        <v>176</v>
+      </c>
+      <c r="G49" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="D50" t="s">
+    <row r="50" spans="1:8">
+      <c r="E50" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" t="s">
+        <v>178</v>
+      </c>
+      <c r="G50" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:8">
       <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="H51" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="D52" s="4" t="s">
+    <row r="52" spans="1:8">
+      <c r="E52" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G52" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="D53" s="1" t="s">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="E53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F53" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E53" t="s">
+      <c r="H53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="D54" s="1" t="s">
+    <row r="54" spans="1:8">
+      <c r="E54" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="D55" s="1" t="s">
+    <row r="55" spans="1:8">
+      <c r="E55" t="s">
+        <v>188</v>
+      </c>
+      <c r="F55" t="s">
+        <v>189</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="D56" s="1" t="s">
+    <row r="56" spans="1:8">
+      <c r="E56" t="s">
+        <v>194</v>
+      </c>
+      <c r="F56" t="s">
+        <v>195</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="D57" s="1" t="s">
+    <row r="57" spans="1:8">
+      <c r="E57" t="s">
+        <v>196</v>
+      </c>
+      <c r="F57" t="s">
+        <v>197</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
-      <c r="D58" s="1" t="s">
+    <row r="58" spans="1:8">
+      <c r="E58" t="s">
+        <v>206</v>
+      </c>
+      <c r="F58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
-      <c r="D59" s="1" t="s">
+    <row r="59" spans="1:8">
+      <c r="E59" t="s">
+        <v>208</v>
+      </c>
+      <c r="F59" t="s">
+        <v>209</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60" s="9" t="s">
         <v>114</v>
       </c>
@@ -1636,138 +2469,255 @@
       <c r="C60" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="H60" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="D61" s="4" t="s">
+    <row r="61" spans="1:8">
+      <c r="E61" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="D62" s="4" t="s">
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="E62" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="D63" s="4" t="s">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="E63" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="4"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="D64" s="2" t="s">
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="E64" t="s">
+        <v>144</v>
+      </c>
+      <c r="F64" t="s">
+        <v>145</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E64" t="s">
+      <c r="H64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="2:5">
-      <c r="D65" s="2" t="s">
+    <row r="65" spans="2:8">
+      <c r="E65" t="s">
+        <v>171</v>
+      </c>
+      <c r="F65" t="s">
+        <v>172</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="2:5">
-      <c r="D66" s="2" t="s">
+    <row r="66" spans="2:8">
+      <c r="E66" t="s">
+        <v>173</v>
+      </c>
+      <c r="F66" t="s">
+        <v>174</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:8">
       <c r="B67" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="G67" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="H67" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="2:5">
-      <c r="D68" s="4" t="s">
+    <row r="68" spans="2:8">
+      <c r="G68" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="D69" s="4" t="s">
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="E69" t="s">
+        <v>223</v>
+      </c>
+      <c r="F69" t="s">
+        <v>224</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="2:5">
-      <c r="D70" s="1" t="s">
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="E70" t="s">
+        <v>132</v>
+      </c>
+      <c r="F70" t="s">
+        <v>133</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E70" t="s">
+      <c r="H70" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="2:5">
-      <c r="D71" s="1" t="s">
+    <row r="71" spans="2:8">
+      <c r="E71" t="s">
+        <v>151</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="2:5">
-      <c r="D72" s="1" t="s">
+    <row r="72" spans="2:8">
+      <c r="E72" t="s">
+        <v>161</v>
+      </c>
+      <c r="F72" t="s">
+        <v>162</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="2:5">
+    <row r="73" spans="2:8">
       <c r="B73" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G73" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="H73" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="2:5">
-      <c r="D74" s="4" t="s">
+    <row r="74" spans="2:8">
+      <c r="E74" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E74" s="4"/>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="D75" s="4" t="s">
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="E75" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="2:5">
-      <c r="D76" s="1" t="s">
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="E76" t="s">
+        <v>135</v>
+      </c>
+      <c r="F76" t="s">
+        <v>136</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E76" t="s">
+      <c r="H76" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="2:5">
-      <c r="D77" s="1" t="s">
+    <row r="77" spans="2:8">
+      <c r="E77" t="s">
+        <v>153</v>
+      </c>
+      <c r="F77" t="s">
+        <v>154</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="2:5">
-      <c r="D78" s="1" t="s">
+    <row r="78" spans="2:8">
+      <c r="E78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="2:5">
+    <row r="79" spans="2:8">
       <c r="B79" s="7" t="s">
         <v>9</v>
       </c>
@@ -1775,28 +2725,37 @@
         <v>64</v>
       </c>
       <c r="D79" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G79" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="H79" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="2:5">
-      <c r="D80" s="1" t="s">
+    <row r="80" spans="2:8">
+      <c r="G80" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="D81" s="1" t="s">
+    <row r="81" spans="1:8">
+      <c r="G81" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="D82" s="1" t="s">
+    <row r="82" spans="1:8">
+      <c r="G82" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:8">
       <c r="B83" s="7" t="s">
         <v>10</v>
       </c>
@@ -1804,25 +2763,43 @@
         <v>49</v>
       </c>
       <c r="D83" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G83" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E83" s="7" t="s">
+      <c r="H83" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
-      <c r="D84" s="1" t="s">
+    <row r="84" spans="1:8">
+      <c r="E84" t="s">
+        <v>221</v>
+      </c>
+      <c r="F84" t="s">
+        <v>222</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:8">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E85" s="5"/>
+      <c r="H85" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>